<commit_message>
change password ok (Patient und Arzt)
</commit_message>
<xml_diff>
--- a/rendezvous.xlsx
+++ b/rendezvous.xlsx
@@ -539,7 +539,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E7" activeCellId="0" sqref="E7"/>
@@ -670,6 +670,72 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Dr. Schmidt</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2023-11-15</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Dr. Schmidt</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2023-11-17</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>14:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Dr. Schmidt</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2023-11-17</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>14:30</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>